<commit_message>
Created pivots in excel as part of the action
</commit_message>
<xml_diff>
--- a/alerts.xlsx
+++ b/alerts.xlsx
@@ -5,6 +5,8 @@
   <sheets>
     <sheet name="code-scanning-issues" sheetId="1" r:id="rId1"/>
     <sheet name="dependencies-list" sheetId="2" r:id="rId2"/>
+    <sheet name="dependencies-Pivot" sheetId="3" r:id="rId3"/>
+    <sheet name="code-scanning-Pivot" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -412,7 +414,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/293</v>
       </c>
       <c r="D2" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E2" t="str">
         <v>java/random-used-once</v>
@@ -432,7 +434,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/292</v>
       </c>
       <c r="D3" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E3" t="str">
         <v>java/potentially-weak-cryptographic-algorithm</v>
@@ -452,7 +454,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/291</v>
       </c>
       <c r="D4" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E4" t="str">
         <v>java/unsafe-get-resource</v>
@@ -472,7 +474,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/290</v>
       </c>
       <c r="D5" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E5" t="str">
         <v>java/unused-parameter</v>
@@ -492,7 +494,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/289</v>
       </c>
       <c r="D6" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E6" t="str">
         <v>java/unused-parameter</v>
@@ -512,7 +514,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/288</v>
       </c>
       <c r="D7" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E7" t="str">
         <v>java/unused-parameter</v>
@@ -532,7 +534,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/287</v>
       </c>
       <c r="D8" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E8" t="str">
         <v>java/unused-parameter</v>
@@ -552,7 +554,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/286</v>
       </c>
       <c r="D9" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E9" t="str">
         <v>java/unused-parameter</v>
@@ -572,7 +574,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/285</v>
       </c>
       <c r="D10" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E10" t="str">
         <v>java/unused-parameter</v>
@@ -592,7 +594,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/284</v>
       </c>
       <c r="D11" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E11" t="str">
         <v>java/unused-parameter</v>
@@ -612,7 +614,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/283</v>
       </c>
       <c r="D12" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E12" t="str">
         <v>java/unused-parameter</v>
@@ -632,7 +634,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/282</v>
       </c>
       <c r="D13" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E13" t="str">
         <v>java/unused-parameter</v>
@@ -652,7 +654,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/281</v>
       </c>
       <c r="D14" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E14" t="str">
         <v>java/unused-parameter</v>
@@ -672,7 +674,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/280</v>
       </c>
       <c r="D15" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E15" t="str">
         <v>java/non-static-nested-class</v>
@@ -692,7 +694,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/279</v>
       </c>
       <c r="D16" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E16" t="str">
         <v>java/non-static-nested-class</v>
@@ -712,7 +714,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/278</v>
       </c>
       <c r="D17" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E17" t="str">
         <v>java/non-static-nested-class</v>
@@ -732,7 +734,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/277</v>
       </c>
       <c r="D18" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E18" t="str">
         <v>java/non-static-nested-class</v>
@@ -752,7 +754,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/276</v>
       </c>
       <c r="D19" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E19" t="str">
         <v>java/non-static-nested-class</v>
@@ -772,7 +774,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/275</v>
       </c>
       <c r="D20" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E20" t="str">
         <v>java/non-static-nested-class</v>
@@ -792,7 +794,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/274</v>
       </c>
       <c r="D21" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E21" t="str">
         <v>java/non-static-nested-class</v>
@@ -812,7 +814,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/273</v>
       </c>
       <c r="D22" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E22" t="str">
         <v>java/non-static-nested-class</v>
@@ -832,7 +834,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/272</v>
       </c>
       <c r="D23" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E23" t="str">
         <v>java/non-static-nested-class</v>
@@ -852,7 +854,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/271</v>
       </c>
       <c r="D24" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E24" t="str">
         <v>java/non-static-nested-class</v>
@@ -872,7 +874,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/270</v>
       </c>
       <c r="D25" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E25" t="str">
         <v>java/inefficient-empty-string-test</v>
@@ -892,7 +894,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/269</v>
       </c>
       <c r="D26" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E26" t="str">
         <v>java/inefficient-empty-string-test</v>
@@ -912,7 +914,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/268</v>
       </c>
       <c r="D27" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E27" t="str">
         <v>java/input-resource-leak</v>
@@ -932,7 +934,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/267</v>
       </c>
       <c r="D28" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E28" t="str">
         <v>java/input-resource-leak</v>
@@ -952,7 +954,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/266</v>
       </c>
       <c r="D29" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E29" t="str">
         <v>java/input-resource-leak</v>
@@ -972,7 +974,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/265</v>
       </c>
       <c r="D30" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E30" t="str">
         <v>java/database-resource-leak</v>
@@ -992,7 +994,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/264</v>
       </c>
       <c r="D31" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E31" t="str">
         <v>java/database-resource-leak</v>
@@ -1012,7 +1014,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/263</v>
       </c>
       <c r="D32" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E32" t="str">
         <v>java/database-resource-leak</v>
@@ -1032,7 +1034,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/262</v>
       </c>
       <c r="D33" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E33" t="str">
         <v>java/database-resource-leak</v>
@@ -1052,7 +1054,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/261</v>
       </c>
       <c r="D34" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E34" t="str">
         <v>java/database-resource-leak</v>
@@ -1072,7 +1074,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/260</v>
       </c>
       <c r="D35" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E35" t="str">
         <v>java/output-resource-leak</v>
@@ -1092,7 +1094,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/259</v>
       </c>
       <c r="D36" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E36" t="str">
         <v>java/output-resource-leak</v>
@@ -1112,7 +1114,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/258</v>
       </c>
       <c r="D37" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E37" t="str">
         <v>java/unused-format-argument</v>
@@ -1132,7 +1134,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/257</v>
       </c>
       <c r="D38" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E38" t="str">
         <v>java/missing-space-in-concatenation</v>
@@ -1152,7 +1154,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/256</v>
       </c>
       <c r="D39" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E39" t="str">
         <v>java/dereferenced-value-may-be-null</v>
@@ -1172,7 +1174,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/255</v>
       </c>
       <c r="D40" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E40" t="str">
         <v>java/local-variable-is-never-read</v>
@@ -1192,7 +1194,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/254</v>
       </c>
       <c r="D41" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E41" t="str">
         <v>java/local-variable-is-never-read</v>
@@ -1212,7 +1214,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/253</v>
       </c>
       <c r="D42" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E42" t="str">
         <v>java/unused-reference-type</v>
@@ -1232,7 +1234,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/252</v>
       </c>
       <c r="D43" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E43" t="str">
         <v>java/unused-reference-type</v>
@@ -1252,7 +1254,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/251</v>
       </c>
       <c r="D44" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E44" t="str">
         <v>java/uncaught-number-format-exception</v>
@@ -1272,7 +1274,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/250</v>
       </c>
       <c r="D45" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E45" t="str">
         <v>java/uncaught-number-format-exception</v>
@@ -1292,7 +1294,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/249</v>
       </c>
       <c r="D46" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E46" t="str">
         <v>java/uncaught-number-format-exception</v>
@@ -1312,7 +1314,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/248</v>
       </c>
       <c r="D47" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E47" t="str">
         <v>java/ignored-error-status-of-call</v>
@@ -1332,7 +1334,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/247</v>
       </c>
       <c r="D48" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E48" t="str">
         <v>java/ignored-error-status-of-call</v>
@@ -1352,7 +1354,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/246</v>
       </c>
       <c r="D49" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E49" t="str">
         <v>java/ignored-error-status-of-call</v>
@@ -1372,7 +1374,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/245</v>
       </c>
       <c r="D50" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E50" t="str">
         <v>java/call-to-object-tostring</v>
@@ -1392,7 +1394,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/244</v>
       </c>
       <c r="D51" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E51" t="str">
         <v>java/deprecated-call</v>
@@ -1412,7 +1414,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/243</v>
       </c>
       <c r="D52" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E52" t="str">
         <v>java/deprecated-call</v>
@@ -1432,7 +1434,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/242</v>
       </c>
       <c r="D53" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E53" t="str">
         <v>java/deprecated-call</v>
@@ -1452,7 +1454,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/241</v>
       </c>
       <c r="D54" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E54" t="str">
         <v>java/deprecated-call</v>
@@ -1472,7 +1474,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/240</v>
       </c>
       <c r="D55" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E55" t="str">
         <v>java/deprecated-call</v>
@@ -1492,7 +1494,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/239</v>
       </c>
       <c r="D56" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E56" t="str">
         <v>java/deprecated-call</v>
@@ -1512,7 +1514,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/238</v>
       </c>
       <c r="D57" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E57" t="str">
         <v>java/missing-override-annotation</v>
@@ -1532,7 +1534,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/237</v>
       </c>
       <c r="D58" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E58" t="str">
         <v>java/missing-override-annotation</v>
@@ -1552,7 +1554,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/236</v>
       </c>
       <c r="D59" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E59" t="str">
         <v>java/missing-override-annotation</v>
@@ -1572,7 +1574,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/235</v>
       </c>
       <c r="D60" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E60" t="str">
         <v>java/missing-override-annotation</v>
@@ -1592,7 +1594,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/234</v>
       </c>
       <c r="D61" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E61" t="str">
         <v>java/missing-override-annotation</v>
@@ -1612,7 +1614,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/233</v>
       </c>
       <c r="D62" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E62" t="str">
         <v>java/missing-override-annotation</v>
@@ -1632,7 +1634,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/232</v>
       </c>
       <c r="D63" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E63" t="str">
         <v>java/missing-override-annotation</v>
@@ -1652,7 +1654,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/231</v>
       </c>
       <c r="D64" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E64" t="str">
         <v>java/missing-override-annotation</v>
@@ -1672,7 +1674,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/230</v>
       </c>
       <c r="D65" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E65" t="str">
         <v>java/missing-override-annotation</v>
@@ -1692,7 +1694,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/229</v>
       </c>
       <c r="D66" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E66" t="str">
         <v>java/missing-override-annotation</v>
@@ -1712,7 +1714,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/228</v>
       </c>
       <c r="D67" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E67" t="str">
         <v>java/missing-override-annotation</v>
@@ -1732,7 +1734,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/227</v>
       </c>
       <c r="D68" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E68" t="str">
         <v>java/missing-override-annotation</v>
@@ -1752,7 +1754,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/226</v>
       </c>
       <c r="D69" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E69" t="str">
         <v>java/missing-override-annotation</v>
@@ -1772,7 +1774,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/225</v>
       </c>
       <c r="D70" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E70" t="str">
         <v>java/missing-override-annotation</v>
@@ -1792,7 +1794,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/224</v>
       </c>
       <c r="D71" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E71" t="str">
         <v>java/missing-override-annotation</v>
@@ -1812,7 +1814,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/223</v>
       </c>
       <c r="D72" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E72" t="str">
         <v>java/missing-override-annotation</v>
@@ -1832,7 +1834,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/222</v>
       </c>
       <c r="D73" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E73" t="str">
         <v>java/missing-override-annotation</v>
@@ -1852,7 +1854,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/221</v>
       </c>
       <c r="D74" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E74" t="str">
         <v>java/path-injection</v>
@@ -1872,7 +1874,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/220</v>
       </c>
       <c r="D75" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E75" t="str">
         <v>java/path-injection</v>
@@ -1892,7 +1894,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/219</v>
       </c>
       <c r="D76" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E76" t="str">
         <v>java/path-injection</v>
@@ -1912,7 +1914,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/218</v>
       </c>
       <c r="D77" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E77" t="str">
         <v>java/path-injection</v>
@@ -1932,7 +1934,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/217</v>
       </c>
       <c r="D78" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E78" t="str">
         <v>java/path-injection</v>
@@ -1952,7 +1954,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/216</v>
       </c>
       <c r="D79" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E79" t="str">
         <v>java/zipslip</v>
@@ -1972,7 +1974,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/215</v>
       </c>
       <c r="D80" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E80" t="str">
         <v>java/spring-disabled-csrf-protection</v>
@@ -1992,7 +1994,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/214</v>
       </c>
       <c r="D81" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E81" t="str">
         <v>java/spring-disabled-csrf-protection</v>
@@ -2012,7 +2014,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/213</v>
       </c>
       <c r="D82" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E82" t="str">
         <v>java/sql-injection</v>
@@ -2032,7 +2034,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/212</v>
       </c>
       <c r="D83" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E83" t="str">
         <v>java/sql-injection</v>
@@ -2052,7 +2054,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/211</v>
       </c>
       <c r="D84" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E84" t="str">
         <v>java/sql-injection</v>
@@ -2072,7 +2074,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/210</v>
       </c>
       <c r="D85" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E85" t="str">
         <v>java/missing-jwt-signature-check</v>
@@ -2092,7 +2094,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/209</v>
       </c>
       <c r="D86" t="str">
-        <v>open</v>
+        <v>fixed</v>
       </c>
       <c r="E86" t="str">
         <v>java/missing-jwt-signature-check</v>
@@ -2632,7 +2634,7 @@
         <v>https://github.com/amitgupta7/WebGoat/security/code-scanning/182</v>
       </c>
       <c r="D113" t="str">
-        <v>fixed</v>
+        <v>open</v>
       </c>
       <c r="E113" t="str">
         <v>java/unused-reference-type</v>
@@ -6270,7 +6272,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7572,16 +7574,16 @@
         <v>.github/workflows/codeql-analysis.yml</v>
       </c>
       <c r="B77" t="str">
-        <v>advanced-security/delombok-action</v>
+        <v>github/codeql-action/analyze</v>
       </c>
       <c r="C77" t="str">
         <v>ACTIONS</v>
       </c>
       <c r="D77" t="str">
-        <v>= webgoat</v>
+        <v>= 1</v>
       </c>
       <c r="E77" t="str">
-        <v/>
+        <v>MIT License</v>
       </c>
     </row>
     <row r="78">
@@ -7589,7 +7591,7 @@
         <v>.github/workflows/codeql-analysis.yml</v>
       </c>
       <c r="B78" t="str">
-        <v>github/codeql-action/analyze</v>
+        <v>github/codeql-action/init</v>
       </c>
       <c r="C78" t="str">
         <v>ACTIONS</v>
@@ -7603,16 +7605,16 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>.github/workflows/codeql-analysis.yml</v>
+        <v>.github/workflows/main.yml</v>
       </c>
       <c r="B79" t="str">
-        <v>github/codeql-action/init</v>
+        <v>actions/upload-artifact</v>
       </c>
       <c r="C79" t="str">
         <v>ACTIONS</v>
       </c>
       <c r="D79" t="str">
-        <v>= 1</v>
+        <v>= 2</v>
       </c>
       <c r="E79" t="str">
         <v>MIT License</v>
@@ -7623,7 +7625,7 @@
         <v>.github/workflows/main.yml</v>
       </c>
       <c r="B80" t="str">
-        <v>actions/upload-artifact</v>
+        <v>amitgupta7/ghas-reports-action</v>
       </c>
       <c r="C80" t="str">
         <v>ACTIONS</v>
@@ -7637,19 +7639,19 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>.github/workflows/main.yml</v>
+        <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B81" t="str">
-        <v>amitgupta7/ghas-reports-action</v>
+        <v>org.apache.commons:commons-lang3</v>
       </c>
       <c r="C81" t="str">
-        <v>ACTIONS</v>
+        <v>MAVEN</v>
       </c>
       <c r="D81" t="str">
-        <v>= 2</v>
+        <v/>
       </c>
       <c r="E81" t="str">
-        <v>MIT License</v>
+        <v>Apache License 2.0</v>
       </c>
     </row>
     <row r="82">
@@ -7657,7 +7659,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B82" t="str">
-        <v>org.apache.commons:commons-lang3</v>
+        <v>org.apache.maven.plugins:maven-jar-plugin</v>
       </c>
       <c r="C82" t="str">
         <v>MAVEN</v>
@@ -7674,7 +7676,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B83" t="str">
-        <v>org.apache.maven.plugins:maven-jar-plugin</v>
+        <v>org.apache.maven.plugins:maven-surefire-plugin</v>
       </c>
       <c r="C83" t="str">
         <v>MAVEN</v>
@@ -7683,7 +7685,7 @@
         <v/>
       </c>
       <c r="E83" t="str">
-        <v>Apache License 2.0</v>
+        <v/>
       </c>
     </row>
     <row r="84">
@@ -7691,7 +7693,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B84" t="str">
-        <v>org.apache.maven.plugins:maven-surefire-plugin</v>
+        <v>org.asciidoctor:asciidoctorj</v>
       </c>
       <c r="C84" t="str">
         <v>MAVEN</v>
@@ -7708,7 +7710,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B85" t="str">
-        <v>org.asciidoctor:asciidoctorj</v>
+        <v>org.flywaydb:flyway-core</v>
       </c>
       <c r="C85" t="str">
         <v>MAVEN</v>
@@ -7717,7 +7719,7 @@
         <v/>
       </c>
       <c r="E85" t="str">
-        <v/>
+        <v>Other</v>
       </c>
     </row>
     <row r="86">
@@ -7725,7 +7727,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B86" t="str">
-        <v>org.flywaydb:flyway-core</v>
+        <v>org.hsqldb:hsqldb</v>
       </c>
       <c r="C86" t="str">
         <v>MAVEN</v>
@@ -7734,7 +7736,7 @@
         <v/>
       </c>
       <c r="E86" t="str">
-        <v>Other</v>
+        <v/>
       </c>
     </row>
     <row r="87">
@@ -7742,7 +7744,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B87" t="str">
-        <v>org.hsqldb:hsqldb</v>
+        <v>org.springframework.boot:spring-boot-starter-actuator</v>
       </c>
       <c r="C87" t="str">
         <v>MAVEN</v>
@@ -7751,7 +7753,7 @@
         <v/>
       </c>
       <c r="E87" t="str">
-        <v/>
+        <v>Apache License 2.0</v>
       </c>
     </row>
     <row r="88">
@@ -7759,7 +7761,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B88" t="str">
-        <v>org.springframework.boot:spring-boot-starter-actuator</v>
+        <v>org.springframework.boot:spring-boot-starter-data-jpa</v>
       </c>
       <c r="C88" t="str">
         <v>MAVEN</v>
@@ -7776,7 +7778,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B89" t="str">
-        <v>org.springframework.boot:spring-boot-starter-data-jpa</v>
+        <v>org.springframework.boot:spring-boot-starter-security</v>
       </c>
       <c r="C89" t="str">
         <v>MAVEN</v>
@@ -7793,7 +7795,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B90" t="str">
-        <v>org.springframework.boot:spring-boot-starter-security</v>
+        <v>org.springframework.boot:spring-boot-starter-test</v>
       </c>
       <c r="C90" t="str">
         <v>MAVEN</v>
@@ -7810,7 +7812,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B91" t="str">
-        <v>org.springframework.boot:spring-boot-starter-test</v>
+        <v>org.springframework.boot:spring-boot-starter-thymeleaf</v>
       </c>
       <c r="C91" t="str">
         <v>MAVEN</v>
@@ -7827,7 +7829,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B92" t="str">
-        <v>org.springframework.boot:spring-boot-starter-thymeleaf</v>
+        <v>org.springframework.boot:spring-boot-starter-undertow</v>
       </c>
       <c r="C92" t="str">
         <v>MAVEN</v>
@@ -7844,7 +7846,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B93" t="str">
-        <v>org.springframework.boot:spring-boot-starter-undertow</v>
+        <v>org.springframework.boot:spring-boot-starter-web</v>
       </c>
       <c r="C93" t="str">
         <v>MAVEN</v>
@@ -7861,7 +7863,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B94" t="str">
-        <v>org.springframework.boot:spring-boot-starter-web</v>
+        <v>org.springframework.security:spring-security-test</v>
       </c>
       <c r="C94" t="str">
         <v>MAVEN</v>
@@ -7878,7 +7880,7 @@
         <v>webgoat-container/pom.xml</v>
       </c>
       <c r="B95" t="str">
-        <v>org.springframework.security:spring-security-test</v>
+        <v>org.thymeleaf.extras:thymeleaf-extras-springsecurity5</v>
       </c>
       <c r="C95" t="str">
         <v>MAVEN</v>
@@ -7887,24 +7889,24 @@
         <v/>
       </c>
       <c r="E95" t="str">
-        <v>Apache License 2.0</v>
+        <v/>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>webgoat-container/pom.xml</v>
+        <v>webgoat-integration-tests/pom.xml</v>
       </c>
       <c r="B96" t="str">
-        <v>org.thymeleaf.extras:thymeleaf-extras-springsecurity5</v>
+        <v>io.github.bonigarcia:webdrivermanager</v>
       </c>
       <c r="C96" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D96" t="str">
-        <v/>
+        <v>= 4.3.1</v>
       </c>
       <c r="E96" t="str">
-        <v/>
+        <v>Apache License 2.0</v>
       </c>
     </row>
     <row r="97">
@@ -7912,13 +7914,13 @@
         <v>webgoat-integration-tests/pom.xml</v>
       </c>
       <c r="B97" t="str">
-        <v>io.github.bonigarcia:webdrivermanager</v>
+        <v>io.rest-assured:rest-assured</v>
       </c>
       <c r="C97" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D97" t="str">
-        <v>= 4.3.1</v>
+        <v/>
       </c>
       <c r="E97" t="str">
         <v>Apache License 2.0</v>
@@ -7929,7 +7931,7 @@
         <v>webgoat-integration-tests/pom.xml</v>
       </c>
       <c r="B98" t="str">
-        <v>io.rest-assured:rest-assured</v>
+        <v>org.apache.maven.plugins:maven-surefire-plugin</v>
       </c>
       <c r="C98" t="str">
         <v>MAVEN</v>
@@ -7938,7 +7940,7 @@
         <v/>
       </c>
       <c r="E98" t="str">
-        <v>Apache License 2.0</v>
+        <v/>
       </c>
     </row>
     <row r="99">
@@ -7946,13 +7948,13 @@
         <v>webgoat-integration-tests/pom.xml</v>
       </c>
       <c r="B99" t="str">
-        <v>org.apache.maven.plugins:maven-surefire-plugin</v>
+        <v>org.owasp.webgoat:webgoat-server</v>
       </c>
       <c r="C99" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D99" t="str">
-        <v/>
+        <v>= 8.2.3-SNAPSHOT</v>
       </c>
       <c r="E99" t="str">
         <v/>
@@ -7963,7 +7965,7 @@
         <v>webgoat-integration-tests/pom.xml</v>
       </c>
       <c r="B100" t="str">
-        <v>org.owasp.webgoat:webgoat-server</v>
+        <v>org.owasp.webgoat:webwolf</v>
       </c>
       <c r="C100" t="str">
         <v>MAVEN</v>
@@ -7980,16 +7982,16 @@
         <v>webgoat-integration-tests/pom.xml</v>
       </c>
       <c r="B101" t="str">
-        <v>org.owasp.webgoat:webwolf</v>
+        <v>org.seleniumhq.selenium:selenium-java</v>
       </c>
       <c r="C101" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D101" t="str">
-        <v>= 8.2.3-SNAPSHOT</v>
+        <v/>
       </c>
       <c r="E101" t="str">
-        <v/>
+        <v>Apache License 2.0</v>
       </c>
     </row>
     <row r="102">
@@ -7997,7 +7999,7 @@
         <v>webgoat-integration-tests/pom.xml</v>
       </c>
       <c r="B102" t="str">
-        <v>org.seleniumhq.selenium:selenium-java</v>
+        <v>org.springframework.boot:spring-boot-starter-test</v>
       </c>
       <c r="C102" t="str">
         <v>MAVEN</v>
@@ -8011,16 +8013,16 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>webgoat-integration-tests/pom.xml</v>
+        <v>webgoat-lessons/challenge/pom.xml</v>
       </c>
       <c r="B103" t="str">
-        <v>org.springframework.boot:spring-boot-starter-test</v>
+        <v>io.jsonwebtoken:jjwt</v>
       </c>
       <c r="C103" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D103" t="str">
-        <v/>
+        <v>= 0.9.1</v>
       </c>
       <c r="E103" t="str">
         <v>Apache License 2.0</v>
@@ -8031,13 +8033,13 @@
         <v>webgoat-lessons/challenge/pom.xml</v>
       </c>
       <c r="B104" t="str">
-        <v>io.jsonwebtoken:jjwt</v>
+        <v>org.springframework.boot:spring-boot-starter-test</v>
       </c>
       <c r="C104" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D104" t="str">
-        <v>= 0.9.1</v>
+        <v/>
       </c>
       <c r="E104" t="str">
         <v>Apache License 2.0</v>
@@ -8048,7 +8050,7 @@
         <v>webgoat-lessons/challenge/pom.xml</v>
       </c>
       <c r="B105" t="str">
-        <v>org.springframework.boot:spring-boot-starter-test</v>
+        <v>org.springframework.security:spring-security-test</v>
       </c>
       <c r="C105" t="str">
         <v>MAVEN</v>
@@ -8062,10 +8064,10 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>webgoat-lessons/challenge/pom.xml</v>
+        <v>webgoat-lessons/http-proxies/pom.xml</v>
       </c>
       <c r="B106" t="str">
-        <v>org.springframework.security:spring-security-test</v>
+        <v>org.springframework.boot:spring-boot-starter-test</v>
       </c>
       <c r="C106" t="str">
         <v>MAVEN</v>
@@ -8082,7 +8084,7 @@
         <v>webgoat-lessons/http-proxies/pom.xml</v>
       </c>
       <c r="B107" t="str">
-        <v>org.springframework.boot:spring-boot-starter-test</v>
+        <v>org.springframework.security:spring-security-test</v>
       </c>
       <c r="C107" t="str">
         <v>MAVEN</v>
@@ -8096,36 +8098,36 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>webgoat-lessons/http-proxies/pom.xml</v>
+        <v>webgoat-lessons/hijack-session/pom.xml</v>
       </c>
       <c r="B108" t="str">
-        <v>org.springframework.security:spring-security-test</v>
+        <v>org.jacoco:jacoco-maven-plugin</v>
       </c>
       <c r="C108" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D108" t="str">
-        <v/>
+        <v>= 0.8.7</v>
       </c>
       <c r="E108" t="str">
-        <v>Apache License 2.0</v>
+        <v>Other</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>webgoat-lessons/hijack-session/pom.xml</v>
+        <v>webgoat-lessons/html-tampering/pom.xml</v>
       </c>
       <c r="B109" t="str">
-        <v>org.jacoco:jacoco-maven-plugin</v>
+        <v>org.springframework.boot:spring-boot-starter-test</v>
       </c>
       <c r="C109" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D109" t="str">
-        <v>= 0.8.7</v>
+        <v/>
       </c>
       <c r="E109" t="str">
-        <v>Other</v>
+        <v>Apache License 2.0</v>
       </c>
     </row>
     <row r="110">
@@ -8133,7 +8135,7 @@
         <v>webgoat-lessons/html-tampering/pom.xml</v>
       </c>
       <c r="B110" t="str">
-        <v>org.springframework.boot:spring-boot-starter-test</v>
+        <v>org.springframework.security:spring-security-test</v>
       </c>
       <c r="C110" t="str">
         <v>MAVEN</v>
@@ -8147,41 +8149,1389 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>webgoat-lessons/html-tampering/pom.xml</v>
+        <v>webgoat-lessons/cross-site-scripting/pom.xml</v>
       </c>
       <c r="B111" t="str">
-        <v>org.springframework.security:spring-security-test</v>
+        <v>org.jsoup:jsoup</v>
       </c>
       <c r="C111" t="str">
         <v>MAVEN</v>
       </c>
       <c r="D111" t="str">
-        <v/>
+        <v>= 1.14.2</v>
       </c>
       <c r="E111" t="str">
-        <v>Apache License 2.0</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="str">
-        <v>webgoat-lessons/cross-site-scripting/pom.xml</v>
-      </c>
-      <c r="B112" t="str">
-        <v>org.jsoup:jsoup</v>
-      </c>
-      <c r="C112" t="str">
-        <v>MAVEN</v>
-      </c>
-      <c r="D112" t="str">
-        <v>= 1.14.2</v>
-      </c>
-      <c r="E112" t="str">
         <v>MIT License</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E112"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E111"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>count packageName</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Other</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Apache License 2.0</v>
+      </c>
+      <c r="D1" t="str">
+        <v/>
+      </c>
+      <c r="E1" t="str">
+        <v>BSD 2-Clause "Simplified" License</v>
+      </c>
+      <c r="F1" t="str">
+        <v>MIT License</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Totals</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>pom.xml</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>docker/pom.xml</v>
+      </c>
+      <c r="B3" t="str">
+        <v/>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>webwolf/pom.xml</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>webgoat-server/pom.xml</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>webgoat-lessons/pom.xml</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>.github/workflows/codeql-analysis.yml</v>
+      </c>
+      <c r="B7" t="str">
+        <v/>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>.github/workflows/main.yml</v>
+      </c>
+      <c r="B8" t="str">
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>webgoat-container/pom.xml</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>webgoat-integration-tests/pom.xml</v>
+      </c>
+      <c r="B10" t="str">
+        <v/>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>webgoat-lessons/challenge/pom.xml</v>
+      </c>
+      <c r="B11" t="str">
+        <v/>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>webgoat-lessons/http-proxies/pom.xml</v>
+      </c>
+      <c r="B12" t="str">
+        <v/>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>webgoat-lessons/hijack-session/pom.xml</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <v/>
+      </c>
+      <c r="E13" t="str">
+        <v/>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>webgoat-lessons/html-tampering/pom.xml</v>
+      </c>
+      <c r="B14" t="str">
+        <v/>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>webgoat-lessons/cross-site-scripting/pom.xml</v>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Totals</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>42</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G16"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>count html_url</v>
+      </c>
+      <c r="B1" t="str">
+        <v>warning</v>
+      </c>
+      <c r="C1" t="str">
+        <v>note</v>
+      </c>
+      <c r="D1" t="str">
+        <v>error</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Totals</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>java/random-used-once</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>java/potentially-weak-cryptographic-algorithm</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>java/unsafe-get-resource</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>java/unused-parameter</v>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>java/non-static-nested-class</v>
+      </c>
+      <c r="B6" t="str">
+        <v/>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>java/inefficient-empty-string-test</v>
+      </c>
+      <c r="B7" t="str">
+        <v/>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>java/input-resource-leak</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>java/database-resource-leak</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>java/output-resource-leak</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>java/unused-format-argument</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="str">
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>java/missing-space-in-concatenation</v>
+      </c>
+      <c r="B12" t="str">
+        <v/>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>java/dereferenced-value-may-be-null</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <v/>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>java/local-variable-is-never-read</v>
+      </c>
+      <c r="B14" t="str">
+        <v/>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>java/unused-reference-type</v>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>java/uncaught-number-format-exception</v>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>java/ignored-error-status-of-call</v>
+      </c>
+      <c r="B17" t="str">
+        <v/>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>java/call-to-object-tostring</v>
+      </c>
+      <c r="B18" t="str">
+        <v/>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>java/deprecated-call</v>
+      </c>
+      <c r="B19" t="str">
+        <v/>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>java/missing-override-annotation</v>
+      </c>
+      <c r="B20" t="str">
+        <v/>
+      </c>
+      <c r="C20">
+        <v>23</v>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
+      <c r="E20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>java/path-injection</v>
+      </c>
+      <c r="B21" t="str">
+        <v/>
+      </c>
+      <c r="C21" t="str">
+        <v/>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>java/zipslip</v>
+      </c>
+      <c r="B22" t="str">
+        <v/>
+      </c>
+      <c r="C22" t="str">
+        <v/>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>java/spring-disabled-csrf-protection</v>
+      </c>
+      <c r="B23" t="str">
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>java/sql-injection</v>
+      </c>
+      <c r="B24" t="str">
+        <v/>
+      </c>
+      <c r="C24" t="str">
+        <v/>
+      </c>
+      <c r="D24">
+        <v>13</v>
+      </c>
+      <c r="E24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>java/missing-jwt-signature-check</v>
+      </c>
+      <c r="B25" t="str">
+        <v/>
+      </c>
+      <c r="C25" t="str">
+        <v/>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>java/concatenated-sql-query</v>
+      </c>
+      <c r="B26" t="str">
+        <v/>
+      </c>
+      <c r="C26" t="str">
+        <v/>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>java/reference-equality-on-strings</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="str">
+        <v/>
+      </c>
+      <c r="D27" t="str">
+        <v/>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>java/multiplication-of-remainder</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="str">
+        <v/>
+      </c>
+      <c r="D28" t="str">
+        <v/>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>java/non-null-boxed-variable</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="str">
+        <v/>
+      </c>
+      <c r="D29" t="str">
+        <v/>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>java/useless-tostring-call</v>
+      </c>
+      <c r="B30" t="str">
+        <v/>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>java/index-out-of-bounds</v>
+      </c>
+      <c r="B31" t="str">
+        <v/>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>java/xxe</v>
+      </c>
+      <c r="B32" t="str">
+        <v/>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>java/insecure-cookie</v>
+      </c>
+      <c r="B33" t="str">
+        <v/>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>java/unsafe-deserialization</v>
+      </c>
+      <c r="B34" t="str">
+        <v/>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>java/stack-trace-exposure</v>
+      </c>
+      <c r="B35" t="str">
+        <v/>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>java/weak-cryptographic-algorithm</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="str">
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <v/>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>java/ssrf</v>
+      </c>
+      <c r="B37" t="str">
+        <v/>
+      </c>
+      <c r="C37" t="str">
+        <v/>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>js/regex/missing-regexp-anchor</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="str">
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <v/>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>js/useless-assignment-to-property</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="str">
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <v/>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>js/unused-local-variable</v>
+      </c>
+      <c r="B40" t="str">
+        <v/>
+      </c>
+      <c r="C40">
+        <v>42</v>
+      </c>
+      <c r="D40" t="str">
+        <v/>
+      </c>
+      <c r="E40">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>js/missing-variable-declaration</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41" t="str">
+        <v/>
+      </c>
+      <c r="D41" t="str">
+        <v/>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>js/useless-assignment-to-local</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42" t="str">
+        <v/>
+      </c>
+      <c r="D42" t="str">
+        <v/>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>js/use-before-declaration</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" t="str">
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <v/>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>js/automatic-semicolon-insertion</v>
+      </c>
+      <c r="B44" t="str">
+        <v/>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" t="str">
+        <v/>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>js/index-out-of-bounds</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="str">
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>js/unknown-directive</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="str">
+        <v/>
+      </c>
+      <c r="D46" t="str">
+        <v/>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>js/unneeded-defensive-code</v>
+      </c>
+      <c r="B47" t="str">
+        <v/>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="str">
+        <v/>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>js/whitespace-contradicts-precedence</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="str">
+        <v/>
+      </c>
+      <c r="D48" t="str">
+        <v/>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>js/useless-expression</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49" t="str">
+        <v/>
+      </c>
+      <c r="D49" t="str">
+        <v/>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>js/trivial-conditional</v>
+      </c>
+      <c r="B50">
+        <v>9</v>
+      </c>
+      <c r="C50" t="str">
+        <v/>
+      </c>
+      <c r="D50" t="str">
+        <v/>
+      </c>
+      <c r="E50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>js/loop-iteration-skipped-due-to-shifting</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="str">
+        <v/>
+      </c>
+      <c r="D51" t="str">
+        <v/>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>js/unused-loop-variable</v>
+      </c>
+      <c r="B52" t="str">
+        <v/>
+      </c>
+      <c r="C52" t="str">
+        <v/>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>js/unsafe-jquery-plugin</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="str">
+        <v/>
+      </c>
+      <c r="D53" t="str">
+        <v/>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>js/html-constructed-from-input</v>
+      </c>
+      <c r="B54" t="str">
+        <v/>
+      </c>
+      <c r="C54" t="str">
+        <v/>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>js/xss-through-dom</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="str">
+        <v/>
+      </c>
+      <c r="D55" t="str">
+        <v/>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>js/incomplete-sanitization</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="str">
+        <v/>
+      </c>
+      <c r="D56" t="str">
+        <v/>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Totals</v>
+      </c>
+      <c r="B57">
+        <v>103</v>
+      </c>
+      <c r="C57">
+        <v>144</v>
+      </c>
+      <c r="D57">
+        <v>46</v>
+      </c>
+      <c r="E57" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E57"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>